<commit_message>
Refatoração: simplificação do gráfico 02 e estrutura em abas
</commit_message>
<xml_diff>
--- a/data/Carga.xlsx
+++ b/data/Carga.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariocabral/Desktop/MeuDashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2338C273-CC91-324E-B72D-495F3E204E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE68FDEE-698E-CF46-AFEF-F9E0444813D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="37420" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acessos" sheetId="1" r:id="rId1"/>
     <sheet name="UsuariosAmbientes" sheetId="2" r:id="rId2"/>
-    <sheet name="Usuarios" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Acessos!$A$1:$G$73</definedName>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="158">
   <si>
     <t>UsuarioID</t>
   </si>
@@ -423,24 +422,6 @@
   </si>
   <si>
     <t>DataConclusaoModulo</t>
-  </si>
-  <si>
-    <t>DataCadastroUsuario</t>
-  </si>
-  <si>
-    <t>16/12/2024 14:45:00</t>
-  </si>
-  <si>
-    <t>04/12/2024 09:32:13</t>
-  </si>
-  <si>
-    <t>04/12/2024 09:31:56</t>
-  </si>
-  <si>
-    <t>04/12/2024 09:31:35</t>
-  </si>
-  <si>
-    <t>16/12/2024 15:45:08</t>
   </si>
   <si>
     <t>DataCadastro</t>
@@ -911,7 +892,7 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2433,7 +2414,7 @@
   <dimension ref="A1:K80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2477,13 +2458,13 @@
         <v>127</v>
       </c>
       <c r="I1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="J1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="K1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -2515,10 +2496,10 @@
         <v>45630</v>
       </c>
       <c r="J2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -2550,10 +2531,10 @@
         <v>45630</v>
       </c>
       <c r="J3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2585,10 +2566,10 @@
         <v>45630</v>
       </c>
       <c r="J4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2614,16 +2595,16 @@
         <v>45630</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I5" s="1">
         <v>45630</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2646,19 +2627,19 @@
         <v>94</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I6" s="1">
         <v>45630</v>
       </c>
       <c r="J6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2681,19 +2662,19 @@
         <v>94</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I7" s="1">
         <v>45630</v>
       </c>
       <c r="J7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -2716,19 +2697,19 @@
         <v>94</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I8" s="1">
         <v>45630</v>
       </c>
       <c r="J8" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -2754,16 +2735,16 @@
         <v>45630</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I9" s="1">
         <v>45630</v>
       </c>
       <c r="J9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -2789,16 +2770,16 @@
         <v>45648</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I10" s="1">
         <v>45630</v>
       </c>
       <c r="J10" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K10" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -2830,10 +2811,10 @@
         <v>45630</v>
       </c>
       <c r="J11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -2865,10 +2846,10 @@
         <v>45630</v>
       </c>
       <c r="J12" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K12" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -2900,10 +2881,10 @@
         <v>45630</v>
       </c>
       <c r="J13" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K13" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -2935,10 +2916,10 @@
         <v>45630</v>
       </c>
       <c r="J14" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K14" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -2970,10 +2951,10 @@
         <v>45630</v>
       </c>
       <c r="J15" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K15" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -3005,10 +2986,10 @@
         <v>45630</v>
       </c>
       <c r="J16" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K16" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -3040,10 +3021,10 @@
         <v>45630</v>
       </c>
       <c r="J17" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -3075,10 +3056,10 @@
         <v>45630</v>
       </c>
       <c r="J18" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K18" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -3110,10 +3091,10 @@
         <v>45630</v>
       </c>
       <c r="J19" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K19" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -3139,16 +3120,16 @@
         <v>45699</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I20" s="1">
         <v>45630</v>
       </c>
       <c r="J20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K20" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -3171,19 +3152,19 @@
         <v>94</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I21" s="1">
         <v>45630</v>
       </c>
       <c r="J21" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K21" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -3215,10 +3196,10 @@
         <v>45630</v>
       </c>
       <c r="J22" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -3241,19 +3222,19 @@
         <v>95</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I23" s="1">
         <v>45630</v>
       </c>
       <c r="J23" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K23" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -3276,19 +3257,19 @@
         <v>95</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I24" s="1">
         <v>45630</v>
       </c>
       <c r="J24" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K24" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -3320,10 +3301,10 @@
         <v>45630</v>
       </c>
       <c r="J25" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K25" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -3355,10 +3336,10 @@
         <v>45630</v>
       </c>
       <c r="J26" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K26" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -3390,10 +3371,10 @@
         <v>45630</v>
       </c>
       <c r="J27" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K27" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -3425,10 +3406,10 @@
         <v>45630</v>
       </c>
       <c r="J28" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K28" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -3460,10 +3441,10 @@
         <v>45630</v>
       </c>
       <c r="J29" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K29" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -3495,10 +3476,10 @@
         <v>45630</v>
       </c>
       <c r="J30" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K30" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -3524,16 +3505,16 @@
         <v>45653</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I31" s="1">
         <v>45630</v>
       </c>
       <c r="J31" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K31" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -3565,10 +3546,10 @@
         <v>45630</v>
       </c>
       <c r="J32" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K32" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -3591,19 +3572,19 @@
         <v>96</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I33" s="1">
         <v>45630</v>
       </c>
       <c r="J33" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K33" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -3626,19 +3607,19 @@
         <v>96</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I34" s="1">
         <v>45630</v>
       </c>
       <c r="J34" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K34" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -3661,19 +3642,19 @@
         <v>96</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I35" s="1">
         <v>45630</v>
       </c>
       <c r="J35" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K35" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -3696,19 +3677,19 @@
         <v>96</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I36" s="1">
         <v>45630</v>
       </c>
       <c r="J36" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K36" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -3731,19 +3712,19 @@
         <v>96</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I37" s="1">
         <v>45630</v>
       </c>
       <c r="J37" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K37" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -3766,19 +3747,19 @@
         <v>96</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I38" s="1">
         <v>45630</v>
       </c>
       <c r="J38" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K38" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -3801,19 +3782,19 @@
         <v>96</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I39" s="1">
         <v>45630</v>
       </c>
       <c r="J39" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K39" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -3836,19 +3817,19 @@
         <v>96</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I40" s="1">
         <v>45630</v>
       </c>
       <c r="J40" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K40" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -3871,19 +3852,19 @@
         <v>96</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I41" s="1">
         <v>45630</v>
       </c>
       <c r="J41" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K41" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -3915,10 +3896,10 @@
         <v>45630</v>
       </c>
       <c r="J42" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K42" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -3950,10 +3931,10 @@
         <v>45630</v>
       </c>
       <c r="J43" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K43" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -3985,10 +3966,10 @@
         <v>45630</v>
       </c>
       <c r="J44" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K44" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -4020,10 +4001,10 @@
         <v>45630</v>
       </c>
       <c r="J45" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K45" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -4055,10 +4036,10 @@
         <v>45630</v>
       </c>
       <c r="J46" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K46" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -4084,16 +4065,16 @@
         <v>45644</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I47" s="1">
         <v>45642</v>
       </c>
       <c r="J47" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K47" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -4119,16 +4100,16 @@
         <v>45646</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I48" s="1">
         <v>45642</v>
       </c>
       <c r="J48" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K48" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -4151,19 +4132,19 @@
         <v>96</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I49" s="1">
         <v>45642</v>
       </c>
       <c r="J49" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K49" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -4189,16 +4170,16 @@
         <v>45706</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I50" s="1">
         <v>45642</v>
       </c>
       <c r="J50" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K50" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -4221,19 +4202,19 @@
         <v>96</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I51" s="1">
         <v>45642</v>
       </c>
       <c r="J51" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K51" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -4259,16 +4240,16 @@
         <v>45647</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I52" s="1">
         <v>45642</v>
       </c>
       <c r="J52" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K52" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -4291,19 +4272,19 @@
         <v>96</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I53" s="1">
         <v>45642</v>
       </c>
       <c r="J53" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K53" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -4326,19 +4307,19 @@
         <v>96</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I54" s="1">
         <v>45642</v>
       </c>
       <c r="J54" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K54" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -4361,19 +4342,19 @@
         <v>96</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I55" s="1">
         <v>45642</v>
       </c>
       <c r="J55" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K55" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -4399,16 +4380,16 @@
         <v>45647</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I56" s="1">
         <v>45642</v>
       </c>
       <c r="J56" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K56" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -4431,19 +4412,19 @@
         <v>96</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I57" s="1">
         <v>45642</v>
       </c>
       <c r="J57" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K57" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -4466,19 +4447,19 @@
         <v>96</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I58" s="1">
         <v>45642</v>
       </c>
       <c r="J58" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K58" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -4501,19 +4482,19 @@
         <v>96</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I59" s="1">
         <v>45642</v>
       </c>
       <c r="J59" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K59" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -4536,19 +4517,19 @@
         <v>96</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I60" s="1">
         <v>45642</v>
       </c>
       <c r="J60" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K60" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -4571,19 +4552,19 @@
         <v>96</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I61" s="1">
         <v>45642</v>
       </c>
       <c r="J61" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K61" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -4609,16 +4590,16 @@
         <v>45644</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I62" s="1">
         <v>45642</v>
       </c>
       <c r="J62" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K62" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -4650,10 +4631,10 @@
         <v>45642</v>
       </c>
       <c r="J63" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K63" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -4676,19 +4657,19 @@
         <v>96</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I64" s="1">
         <v>45642</v>
       </c>
       <c r="J64" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K64" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -4714,16 +4695,16 @@
         <v>45647</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I65" s="1">
         <v>45642</v>
       </c>
       <c r="J65" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K65" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
@@ -4749,16 +4730,16 @@
         <v>45647</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I66" s="1">
         <v>45642</v>
       </c>
       <c r="J66" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K66" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -4781,19 +4762,19 @@
         <v>95</v>
       </c>
       <c r="G67" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I67" s="1">
         <v>45642</v>
       </c>
       <c r="J67" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K67" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -4816,19 +4797,19 @@
         <v>95</v>
       </c>
       <c r="G68" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I68" s="1">
         <v>45642</v>
       </c>
       <c r="J68" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K68" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -4851,19 +4832,19 @@
         <v>95</v>
       </c>
       <c r="G69" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I69" s="1">
         <v>45642</v>
       </c>
       <c r="J69" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K69" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -4886,19 +4867,19 @@
         <v>95</v>
       </c>
       <c r="G70" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I70" s="1">
         <v>45642</v>
       </c>
       <c r="J70" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K70" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -4921,19 +4902,19 @@
         <v>95</v>
       </c>
       <c r="G71" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I71" s="1">
         <v>45642</v>
       </c>
       <c r="J71" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K71" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -4956,19 +4937,19 @@
         <v>95</v>
       </c>
       <c r="G72" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I72" s="1">
         <v>45642</v>
       </c>
       <c r="J72" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K72" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -4991,19 +4972,19 @@
         <v>95</v>
       </c>
       <c r="G73" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I73" s="1">
         <v>45642</v>
       </c>
       <c r="J73" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K73" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -5026,19 +5007,19 @@
         <v>95</v>
       </c>
       <c r="G74" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I74" s="1">
         <v>45642</v>
       </c>
       <c r="J74" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K74" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -5061,19 +5042,19 @@
         <v>95</v>
       </c>
       <c r="G75" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I75" s="1">
         <v>45642</v>
       </c>
       <c r="J75" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K75" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -5096,19 +5077,19 @@
         <v>94</v>
       </c>
       <c r="G76" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I76" s="1">
         <v>45642</v>
       </c>
       <c r="J76" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K76" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -5131,19 +5112,19 @@
         <v>94</v>
       </c>
       <c r="G77" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I77" s="1">
         <v>45642</v>
       </c>
       <c r="J77" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K77" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -5166,19 +5147,19 @@
         <v>96</v>
       </c>
       <c r="G78" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I78" s="1">
         <v>45642</v>
       </c>
       <c r="J78" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K78" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -5201,19 +5182,19 @@
         <v>96</v>
       </c>
       <c r="G79" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I79" s="1">
         <v>45642</v>
       </c>
       <c r="J79" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K79" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
@@ -5236,90 +5217,23 @@
         <v>96</v>
       </c>
       <c r="G80" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I80" s="1">
         <v>45642</v>
       </c>
       <c r="J80" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K80" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H80" xr:uid="{4DEF9A41-F379-1F49-B5CE-AAD7CB2EE5A6}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06955044-8D82-294A-95A1-12D8D3E499A2}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1424749</v>
-      </c>
-      <c r="B2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1421048</v>
-      </c>
-      <c r="B3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1421047</v>
-      </c>
-      <c r="B4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1421046</v>
-      </c>
-      <c r="B5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1424775</v>
-      </c>
-      <c r="B6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Melhorias nos tooltips, textos descritivos e visual dos relatórios do dashboard
</commit_message>
<xml_diff>
--- a/data/Carga.xlsx
+++ b/data/Carga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariocabral/Desktop/MeuDashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE68FDEE-698E-CF46-AFEF-F9E0444813D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E538DA5E-B6D8-584C-858F-F113CE91D576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="37420" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Acessos!$A$1:$G$73</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">UsuariosAmbientes!$A$1:$H$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">UsuariosAmbientes!$A$1:$K$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="178">
   <si>
     <t>UsuarioID</t>
   </si>
@@ -424,9 +424,6 @@
     <t>DataConclusaoModulo</t>
   </si>
   <si>
-    <t>DataCadastro</t>
-  </si>
-  <si>
     <t>StatusModulo</t>
   </si>
   <si>
@@ -487,9 +484,6 @@
     <t>0:00:15</t>
   </si>
   <si>
-    <t>0:00:40</t>
-  </si>
-  <si>
     <t>Não Iniciado</t>
   </si>
   <si>
@@ -512,6 +506,72 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>RealizadoDentroDoPrazo</t>
+  </si>
+  <si>
+    <t>Dentro do Prazo</t>
+  </si>
+  <si>
+    <t>Trilha 8 - Todos Status de Módulo</t>
+  </si>
+  <si>
+    <t>Trilha 8 - Todos Status de Módulo - Aprovado</t>
+  </si>
+  <si>
+    <t>0:00:25</t>
+  </si>
+  <si>
+    <t>Trilha 8 - Todos Status de Módulo - Aprovado Fora do Prazo</t>
+  </si>
+  <si>
+    <t>Fora do Prazo</t>
+  </si>
+  <si>
+    <t>0:00:22</t>
+  </si>
+  <si>
+    <t>Trilha 8 - Todos Status de Módulo - Reprovado</t>
+  </si>
+  <si>
+    <t>Trilha 8 - Todos Status de Módulo - Reprovado Fora do Prazo</t>
+  </si>
+  <si>
+    <t>0:00:20</t>
+  </si>
+  <si>
+    <t>Trilha 8 - Todos Status de Módulo - Expirado (Não Realizado)</t>
+  </si>
+  <si>
+    <t>Trilha 8 - Todos Status de Módulo - Aguardando Correção</t>
+  </si>
+  <si>
+    <t>Aguardando Correção</t>
+  </si>
+  <si>
+    <t>Trilha 8 - Todos Status de Módulo - Não Liberado</t>
+  </si>
+  <si>
+    <t>Não Liberado</t>
+  </si>
+  <si>
+    <t>Trilha 8 - Todos Status de Módulo - Dispensado</t>
+  </si>
+  <si>
+    <t>Dispensado</t>
+  </si>
+  <si>
+    <t>0:00:50</t>
+  </si>
+  <si>
+    <t>0:02:52</t>
+  </si>
+  <si>
+    <t>9:06:21</t>
+  </si>
+  <si>
+    <t>0:04:58</t>
   </si>
 </sst>
 </file>
@@ -892,7 +952,7 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2397,11 +2457,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G73" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G73">
-      <sortCondition ref="C1:C73"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:G73" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
     <ignoredError sqref="A1:G1" numberStoredAsText="1"/>
@@ -2411,10 +2467,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DEF9A41-F379-1F49-B5CE-AAD7CB2EE5A6}">
-  <dimension ref="A1:K80"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2427,9 +2484,9 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -2451,7 +2508,7 @@
       <c r="F1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>126</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2464,10 +2521,10 @@
         <v>129</v>
       </c>
       <c r="K1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1421046</v>
       </c>
@@ -2492,17 +2549,17 @@
       <c r="H2" s="1">
         <v>45630</v>
       </c>
-      <c r="I2" s="1">
-        <v>45630</v>
+      <c r="I2" t="s">
+        <v>130</v>
       </c>
       <c r="J2" t="s">
         <v>131</v>
       </c>
       <c r="K2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1421046</v>
       </c>
@@ -2527,17 +2584,17 @@
       <c r="H3" s="1">
         <v>45630</v>
       </c>
-      <c r="I3" s="1">
-        <v>45630</v>
+      <c r="I3" t="s">
+        <v>130</v>
       </c>
       <c r="J3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1421046</v>
       </c>
@@ -2562,17 +2619,17 @@
       <c r="H4" s="1">
         <v>45630</v>
       </c>
-      <c r="I4" s="1">
-        <v>45630</v>
+      <c r="I4" t="s">
+        <v>130</v>
       </c>
       <c r="J4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1421046</v>
       </c>
@@ -2595,19 +2652,16 @@
         <v>45630</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I5" s="1">
-        <v>45630</v>
+        <v>155</v>
+      </c>
+      <c r="I5" t="s">
+        <v>136</v>
       </c>
       <c r="J5" t="s">
         <v>135</v>
       </c>
-      <c r="K5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1421046</v>
       </c>
@@ -2627,22 +2681,19 @@
         <v>94</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I6" s="1">
-        <v>45630</v>
+        <v>155</v>
+      </c>
+      <c r="I6" t="s">
+        <v>136</v>
       </c>
       <c r="J6" t="s">
         <v>137</v>
       </c>
-      <c r="K6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1421046</v>
       </c>
@@ -2662,22 +2713,19 @@
         <v>94</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I7" s="1">
-        <v>45630</v>
+        <v>155</v>
+      </c>
+      <c r="I7" t="s">
+        <v>136</v>
       </c>
       <c r="J7" t="s">
         <v>137</v>
       </c>
-      <c r="K7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1421046</v>
       </c>
@@ -2697,22 +2745,19 @@
         <v>94</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I8" s="1">
-        <v>45630</v>
+        <v>155</v>
+      </c>
+      <c r="I8" t="s">
+        <v>136</v>
       </c>
       <c r="J8" t="s">
         <v>137</v>
       </c>
-      <c r="K8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1421046</v>
       </c>
@@ -2735,19 +2780,16 @@
         <v>45630</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I9" s="1">
-        <v>45630</v>
+        <v>155</v>
+      </c>
+      <c r="I9" t="s">
+        <v>136</v>
       </c>
       <c r="J9" t="s">
         <v>137</v>
       </c>
-      <c r="K9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1421046</v>
       </c>
@@ -2770,19 +2812,16 @@
         <v>45648</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I10" s="1">
-        <v>45630</v>
+        <v>155</v>
+      </c>
+      <c r="I10" t="s">
+        <v>136</v>
       </c>
       <c r="J10" t="s">
         <v>137</v>
       </c>
-      <c r="K10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1421046</v>
       </c>
@@ -2807,17 +2846,17 @@
       <c r="H11" s="1">
         <v>45649</v>
       </c>
-      <c r="I11" s="1">
-        <v>45630</v>
+      <c r="I11" t="s">
+        <v>138</v>
       </c>
       <c r="J11" t="s">
         <v>139</v>
       </c>
       <c r="K11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1421046</v>
       </c>
@@ -2842,17 +2881,17 @@
       <c r="H12" s="1">
         <v>45649</v>
       </c>
-      <c r="I12" s="1">
-        <v>45630</v>
+      <c r="I12" t="s">
+        <v>138</v>
       </c>
       <c r="J12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1421046</v>
       </c>
@@ -2877,17 +2916,17 @@
       <c r="H13" s="1">
         <v>45649</v>
       </c>
-      <c r="I13" s="1">
-        <v>45630</v>
+      <c r="I13" t="s">
+        <v>138</v>
       </c>
       <c r="J13" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="K13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1421046</v>
       </c>
@@ -2912,17 +2951,17 @@
       <c r="H14" s="1">
         <v>45649</v>
       </c>
-      <c r="I14" s="1">
-        <v>45630</v>
+      <c r="I14" t="s">
+        <v>138</v>
       </c>
       <c r="J14" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="K14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1421046</v>
       </c>
@@ -2947,17 +2986,17 @@
       <c r="H15" s="1">
         <v>45649</v>
       </c>
-      <c r="I15" s="1">
-        <v>45630</v>
+      <c r="I15" t="s">
+        <v>138</v>
       </c>
       <c r="J15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K15" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1421046</v>
       </c>
@@ -2982,17 +3021,17 @@
       <c r="H16" s="1">
         <v>45649</v>
       </c>
-      <c r="I16" s="1">
-        <v>45630</v>
+      <c r="I16" t="s">
+        <v>138</v>
       </c>
       <c r="J16" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="K16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1421046</v>
       </c>
@@ -3017,17 +3056,17 @@
       <c r="H17" s="1">
         <v>45646</v>
       </c>
-      <c r="I17" s="1">
-        <v>45630</v>
+      <c r="I17" t="s">
+        <v>130</v>
       </c>
       <c r="J17" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="K17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1421046</v>
       </c>
@@ -3052,17 +3091,17 @@
       <c r="H18" s="1">
         <v>45658</v>
       </c>
-      <c r="I18" s="1">
-        <v>45630</v>
+      <c r="I18" t="s">
+        <v>130</v>
       </c>
       <c r="J18" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="K18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1421046</v>
       </c>
@@ -3087,17 +3126,17 @@
       <c r="H19" s="1">
         <v>45642</v>
       </c>
-      <c r="I19" s="1">
-        <v>45630</v>
+      <c r="I19" t="s">
+        <v>130</v>
       </c>
       <c r="J19" t="s">
         <v>131</v>
       </c>
       <c r="K19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1421046</v>
       </c>
@@ -3120,19 +3159,19 @@
         <v>45699</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I20" s="1">
-        <v>45630</v>
+        <v>155</v>
+      </c>
+      <c r="I20" t="s">
+        <v>148</v>
       </c>
       <c r="J20" t="s">
         <v>137</v>
       </c>
       <c r="K20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1421046</v>
       </c>
@@ -3152,24 +3191,21 @@
         <v>94</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I21" s="1">
-        <v>45630</v>
+        <v>155</v>
+      </c>
+      <c r="I21" t="s">
+        <v>136</v>
       </c>
       <c r="J21" t="s">
         <v>137</v>
-      </c>
-      <c r="K21" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1421047</v>
+        <v>1421046</v>
       </c>
       <c r="B22" t="s">
         <v>100</v>
@@ -3178,33 +3214,33 @@
         <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="E22" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="F22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G22" s="1">
-        <v>45630</v>
+        <v>45810</v>
       </c>
       <c r="H22" s="1">
-        <v>45630</v>
-      </c>
-      <c r="I22" s="1">
-        <v>45630</v>
+        <v>45810</v>
+      </c>
+      <c r="I22" t="s">
+        <v>130</v>
       </c>
       <c r="J22" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="K22" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1421047</v>
+        <v>1421046</v>
       </c>
       <c r="B23" t="s">
         <v>100</v>
@@ -3213,33 +3249,33 @@
         <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="E23" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="F23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I23" s="1">
-        <v>45630</v>
+        <v>94</v>
+      </c>
+      <c r="G23" s="1">
+        <v>45810</v>
+      </c>
+      <c r="H23" s="1">
+        <v>45810</v>
+      </c>
+      <c r="I23" t="s">
+        <v>162</v>
       </c>
       <c r="J23" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="K23" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1421047</v>
+        <v>1421046</v>
       </c>
       <c r="B24" t="s">
         <v>100</v>
@@ -3248,33 +3284,33 @@
         <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="F24" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="1">
+        <v>45810</v>
+      </c>
+      <c r="H24" s="1">
+        <v>45810</v>
+      </c>
+      <c r="I24" t="s">
+        <v>138</v>
+      </c>
+      <c r="J24" t="s">
+        <v>139</v>
+      </c>
+      <c r="K24" t="s">
         <v>157</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I24" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J24" t="s">
-        <v>137</v>
-      </c>
-      <c r="K24" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1421047</v>
+        <v>1421046</v>
       </c>
       <c r="B25" t="s">
         <v>100</v>
@@ -3283,33 +3319,33 @@
         <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25" s="1">
-        <v>45630</v>
+        <v>45810</v>
       </c>
       <c r="H25" s="1">
-        <v>45630</v>
-      </c>
-      <c r="I25" s="1">
-        <v>45630</v>
+        <v>45810</v>
+      </c>
+      <c r="I25" t="s">
+        <v>162</v>
       </c>
       <c r="J25" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="K25" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1421047</v>
+        <v>1421046</v>
       </c>
       <c r="B26" t="s">
         <v>100</v>
@@ -3318,33 +3354,30 @@
         <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="F26" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="1">
-        <v>45630</v>
-      </c>
-      <c r="H26" s="1">
-        <v>45630</v>
-      </c>
-      <c r="I26" s="1">
-        <v>45630</v>
+        <v>94</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I26" t="s">
+        <v>136</v>
       </c>
       <c r="J26" t="s">
-        <v>131</v>
-      </c>
-      <c r="K26" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>1421047</v>
+        <v>1421046</v>
       </c>
       <c r="B27" t="s">
         <v>100</v>
@@ -3353,33 +3386,30 @@
         <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="F27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G27" s="1">
-        <v>45630</v>
-      </c>
-      <c r="H27" s="1">
-        <v>45630</v>
-      </c>
-      <c r="I27" s="1">
-        <v>45630</v>
+        <v>45810</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I27" t="s">
+        <v>169</v>
       </c>
       <c r="J27" t="s">
-        <v>131</v>
-      </c>
-      <c r="K27" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>1421047</v>
+        <v>1421046</v>
       </c>
       <c r="B28" t="s">
         <v>100</v>
@@ -3388,33 +3418,30 @@
         <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="E28" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="F28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G28" s="1">
-        <v>45630</v>
-      </c>
-      <c r="H28" s="1">
-        <v>45630</v>
-      </c>
-      <c r="I28" s="1">
-        <v>45630</v>
+        <v>94</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I28" t="s">
+        <v>171</v>
       </c>
       <c r="J28" t="s">
-        <v>131</v>
-      </c>
-      <c r="K28" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>1421047</v>
+        <v>1421046</v>
       </c>
       <c r="B29" t="s">
         <v>100</v>
@@ -3423,31 +3450,28 @@
         <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="F29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G29" s="1">
-        <v>45630</v>
-      </c>
-      <c r="H29" s="1">
-        <v>45630</v>
-      </c>
-      <c r="I29" s="1">
-        <v>45630</v>
+        <v>94</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I29" t="s">
+        <v>173</v>
       </c>
       <c r="J29" t="s">
-        <v>131</v>
-      </c>
-      <c r="K29" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1421047</v>
       </c>
@@ -3461,7 +3485,7 @@
         <v>101</v>
       </c>
       <c r="E30" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F30" t="s">
         <v>95</v>
@@ -3472,17 +3496,17 @@
       <c r="H30" s="1">
         <v>45630</v>
       </c>
-      <c r="I30" s="1">
-        <v>45630</v>
+      <c r="I30" t="s">
+        <v>130</v>
       </c>
       <c r="J30" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="K30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1421047</v>
       </c>
@@ -3493,31 +3517,28 @@
         <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E31" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="F31" t="s">
         <v>95</v>
       </c>
-      <c r="G31" s="1">
-        <v>45653</v>
+      <c r="G31" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I31" s="1">
-        <v>45630</v>
+        <v>155</v>
+      </c>
+      <c r="I31" t="s">
+        <v>136</v>
       </c>
       <c r="J31" t="s">
         <v>137</v>
       </c>
-      <c r="K31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1421047</v>
       </c>
@@ -3528,33 +3549,30 @@
         <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E32" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="F32" t="s">
         <v>95</v>
       </c>
-      <c r="G32" s="1">
-        <v>45642</v>
-      </c>
-      <c r="H32" s="1">
-        <v>45658</v>
-      </c>
-      <c r="I32" s="1">
-        <v>45630</v>
+      <c r="G32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I32" t="s">
+        <v>136</v>
       </c>
       <c r="J32" t="s">
-        <v>131</v>
-      </c>
-      <c r="K32" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1421048</v>
+        <v>1421047</v>
       </c>
       <c r="B33" t="s">
         <v>100</v>
@@ -3566,30 +3584,30 @@
         <v>101</v>
       </c>
       <c r="E33" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="1">
+        <v>45630</v>
+      </c>
+      <c r="H33" s="1">
+        <v>45630</v>
+      </c>
+      <c r="I33" t="s">
+        <v>130</v>
+      </c>
+      <c r="J33" t="s">
+        <v>145</v>
+      </c>
+      <c r="K33" t="s">
         <v>157</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I33" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J33" t="s">
-        <v>150</v>
-      </c>
-      <c r="K33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1421048</v>
+        <v>1421047</v>
       </c>
       <c r="B34" t="s">
         <v>100</v>
@@ -3601,30 +3619,30 @@
         <v>101</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F34" t="s">
-        <v>96</v>
-      </c>
-      <c r="G34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G34" s="1">
+        <v>45630</v>
+      </c>
+      <c r="H34" s="1">
+        <v>45630</v>
+      </c>
+      <c r="I34" t="s">
+        <v>130</v>
+      </c>
+      <c r="J34" t="s">
+        <v>141</v>
+      </c>
+      <c r="K34" t="s">
         <v>157</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I34" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J34" t="s">
-        <v>137</v>
-      </c>
-      <c r="K34" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1421048</v>
+        <v>1421047</v>
       </c>
       <c r="B35" t="s">
         <v>100</v>
@@ -3636,30 +3654,30 @@
         <v>101</v>
       </c>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F35" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G35" s="1">
+        <v>45630</v>
+      </c>
+      <c r="H35" s="1">
+        <v>45630</v>
+      </c>
+      <c r="I35" t="s">
+        <v>130</v>
+      </c>
+      <c r="J35" t="s">
+        <v>146</v>
+      </c>
+      <c r="K35" t="s">
         <v>157</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I35" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J35" t="s">
-        <v>137</v>
-      </c>
-      <c r="K35" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>1421048</v>
+        <v>1421047</v>
       </c>
       <c r="B36" t="s">
         <v>100</v>
@@ -3671,30 +3689,30 @@
         <v>101</v>
       </c>
       <c r="E36" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F36" t="s">
-        <v>96</v>
-      </c>
-      <c r="G36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36" s="1">
+        <v>45630</v>
+      </c>
+      <c r="H36" s="1">
+        <v>45630</v>
+      </c>
+      <c r="I36" t="s">
+        <v>130</v>
+      </c>
+      <c r="J36" t="s">
+        <v>144</v>
+      </c>
+      <c r="K36" t="s">
         <v>157</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I36" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J36" t="s">
-        <v>150</v>
-      </c>
-      <c r="K36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1421048</v>
+        <v>1421047</v>
       </c>
       <c r="B37" t="s">
         <v>100</v>
@@ -3706,30 +3724,30 @@
         <v>101</v>
       </c>
       <c r="E37" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F37" t="s">
-        <v>96</v>
-      </c>
-      <c r="G37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" s="1">
+        <v>45630</v>
+      </c>
+      <c r="H37" s="1">
+        <v>45630</v>
+      </c>
+      <c r="I37" t="s">
+        <v>130</v>
+      </c>
+      <c r="J37" t="s">
+        <v>137</v>
+      </c>
+      <c r="K37" t="s">
         <v>157</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I37" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J37" t="s">
-        <v>137</v>
-      </c>
-      <c r="K37" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>1421048</v>
+        <v>1421047</v>
       </c>
       <c r="B38" t="s">
         <v>100</v>
@@ -3741,170 +3759,164 @@
         <v>101</v>
       </c>
       <c r="E38" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F38" t="s">
-        <v>96</v>
-      </c>
-      <c r="G38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="1">
+        <v>45630</v>
+      </c>
+      <c r="H38" s="1">
+        <v>45630</v>
+      </c>
+      <c r="I38" t="s">
+        <v>130</v>
+      </c>
+      <c r="J38" t="s">
+        <v>147</v>
+      </c>
+      <c r="K38" t="s">
         <v>157</v>
       </c>
-      <c r="H38" s="1" t="s">
+    </row>
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1421047</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" s="1">
+        <v>45653</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I39" t="s">
+        <v>136</v>
+      </c>
+      <c r="J39" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1421047</v>
+      </c>
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" t="s">
+        <v>95</v>
+      </c>
+      <c r="G40" s="1">
+        <v>45642</v>
+      </c>
+      <c r="H40" s="1">
+        <v>45658</v>
+      </c>
+      <c r="I40" t="s">
+        <v>130</v>
+      </c>
+      <c r="J40" t="s">
+        <v>137</v>
+      </c>
+      <c r="K40" t="s">
         <v>157</v>
       </c>
-      <c r="I38" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J38" t="s">
-        <v>137</v>
-      </c>
-      <c r="K38" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>1421048</v>
-      </c>
-      <c r="B39" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" t="s">
-        <v>91</v>
-      </c>
-      <c r="D39" t="s">
-        <v>101</v>
-      </c>
-      <c r="E39" t="s">
-        <v>108</v>
-      </c>
-      <c r="F39" t="s">
-        <v>96</v>
-      </c>
-      <c r="G39" s="1" t="s">
+    </row>
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1421047</v>
+      </c>
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" t="s">
+        <v>122</v>
+      </c>
+      <c r="F41" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I41" t="s">
+        <v>136</v>
+      </c>
+      <c r="J41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1421047</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" t="s">
+        <v>95</v>
+      </c>
+      <c r="G42" s="1">
+        <v>45810</v>
+      </c>
+      <c r="H42" s="1">
+        <v>45810</v>
+      </c>
+      <c r="I42" t="s">
+        <v>130</v>
+      </c>
+      <c r="J42" t="s">
+        <v>144</v>
+      </c>
+      <c r="K42" t="s">
         <v>157</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I39" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J39" t="s">
-        <v>137</v>
-      </c>
-      <c r="K39" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>1421048</v>
-      </c>
-      <c r="B40" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" t="s">
-        <v>109</v>
-      </c>
-      <c r="F40" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I40" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J40" t="s">
-        <v>137</v>
-      </c>
-      <c r="K40" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>1421048</v>
-      </c>
-      <c r="B41" t="s">
-        <v>100</v>
-      </c>
-      <c r="C41" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" t="s">
-        <v>110</v>
-      </c>
-      <c r="F41" t="s">
-        <v>96</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I41" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J41" t="s">
-        <v>137</v>
-      </c>
-      <c r="K41" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>1421048</v>
-      </c>
-      <c r="B42" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" t="s">
-        <v>118</v>
-      </c>
-      <c r="E42" t="s">
-        <v>119</v>
-      </c>
-      <c r="F42" t="s">
-        <v>96</v>
-      </c>
-      <c r="G42" s="1">
-        <v>45647</v>
-      </c>
-      <c r="H42" s="1">
-        <v>45647</v>
-      </c>
-      <c r="I42" s="1">
-        <v>45630</v>
-      </c>
-      <c r="J42" t="s">
-        <v>131</v>
-      </c>
-      <c r="K42" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>1421048</v>
+        <v>1421047</v>
       </c>
       <c r="B43" t="s">
         <v>100</v>
@@ -3913,31 +3925,31 @@
         <v>91</v>
       </c>
       <c r="D43" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E43" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G43" s="1">
-        <v>45642</v>
+        <v>45810</v>
       </c>
       <c r="H43" s="1">
-        <v>45658</v>
-      </c>
-      <c r="I43" s="1">
-        <v>45630</v>
+        <v>45810</v>
+      </c>
+      <c r="I43" t="s">
+        <v>162</v>
       </c>
       <c r="J43" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="K43" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1421048</v>
       </c>
@@ -3948,31 +3960,31 @@
         <v>91</v>
       </c>
       <c r="D44" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="E44" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="F44" t="s">
         <v>96</v>
       </c>
-      <c r="G44" s="1">
-        <v>45647</v>
-      </c>
-      <c r="H44" s="1">
-        <v>45647</v>
-      </c>
-      <c r="I44" s="1">
-        <v>45630</v>
+      <c r="G44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I44" t="s">
+        <v>148</v>
       </c>
       <c r="J44" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="K44" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1421048</v>
       </c>
@@ -3983,31 +3995,28 @@
         <v>91</v>
       </c>
       <c r="D45" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="E45" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="F45" t="s">
         <v>96</v>
       </c>
-      <c r="G45" s="1">
-        <v>45647</v>
-      </c>
-      <c r="H45" s="1">
-        <v>45647</v>
-      </c>
-      <c r="I45" s="1">
-        <v>45630</v>
+      <c r="G45" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I45" t="s">
+        <v>136</v>
       </c>
       <c r="J45" t="s">
-        <v>131</v>
-      </c>
-      <c r="K45" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1421048</v>
       </c>
@@ -4018,33 +4027,30 @@
         <v>91</v>
       </c>
       <c r="D46" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="E46" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="F46" t="s">
         <v>96</v>
       </c>
-      <c r="G46" s="1">
-        <v>45647</v>
-      </c>
-      <c r="H46" s="1">
-        <v>45647</v>
-      </c>
-      <c r="I46" s="1">
-        <v>45630</v>
+      <c r="G46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I46" t="s">
+        <v>136</v>
       </c>
       <c r="J46" t="s">
-        <v>139</v>
-      </c>
-      <c r="K46" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B47" t="s">
         <v>100</v>
@@ -4056,30 +4062,27 @@
         <v>101</v>
       </c>
       <c r="E47" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F47" t="s">
         <v>96</v>
       </c>
-      <c r="G47" s="1">
-        <v>45644</v>
+      <c r="G47" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I47" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I47" t="s">
+        <v>136</v>
       </c>
       <c r="J47" t="s">
-        <v>135</v>
-      </c>
-      <c r="K47" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B48" t="s">
         <v>100</v>
@@ -4091,30 +4094,27 @@
         <v>101</v>
       </c>
       <c r="E48" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F48" t="s">
         <v>96</v>
       </c>
-      <c r="G48" s="1">
-        <v>45646</v>
+      <c r="G48" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I48" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I48" t="s">
+        <v>136</v>
       </c>
       <c r="J48" t="s">
         <v>137</v>
       </c>
-      <c r="K48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B49" t="s">
         <v>100</v>
@@ -4126,30 +4126,27 @@
         <v>101</v>
       </c>
       <c r="E49" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F49" t="s">
         <v>96</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I49" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I49" t="s">
+        <v>136</v>
       </c>
       <c r="J49" t="s">
         <v>137</v>
       </c>
-      <c r="K49" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B50" t="s">
         <v>100</v>
@@ -4161,30 +4158,27 @@
         <v>101</v>
       </c>
       <c r="E50" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F50" t="s">
         <v>96</v>
       </c>
-      <c r="G50" s="1">
-        <v>45706</v>
+      <c r="G50" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I50" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I50" t="s">
+        <v>136</v>
       </c>
       <c r="J50" t="s">
-        <v>135</v>
-      </c>
-      <c r="K50" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B51" t="s">
         <v>100</v>
@@ -4196,30 +4190,27 @@
         <v>101</v>
       </c>
       <c r="E51" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F51" t="s">
         <v>96</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I51" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I51" t="s">
+        <v>136</v>
       </c>
       <c r="J51" t="s">
         <v>137</v>
       </c>
-      <c r="K51" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B52" t="s">
         <v>100</v>
@@ -4231,30 +4222,27 @@
         <v>101</v>
       </c>
       <c r="E52" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F52" t="s">
         <v>96</v>
       </c>
-      <c r="G52" s="1">
-        <v>45647</v>
+      <c r="G52" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I52" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I52" t="s">
+        <v>136</v>
       </c>
       <c r="J52" t="s">
         <v>137</v>
       </c>
-      <c r="K52" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B53" t="s">
         <v>100</v>
@@ -4263,33 +4251,33 @@
         <v>91</v>
       </c>
       <c r="D53" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="E53" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="F53" t="s">
         <v>96</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="G53" s="1">
+        <v>45647</v>
+      </c>
+      <c r="H53" s="1">
+        <v>45647</v>
+      </c>
+      <c r="I53" t="s">
+        <v>130</v>
+      </c>
+      <c r="J53" t="s">
+        <v>131</v>
+      </c>
+      <c r="K53" t="s">
         <v>157</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I53" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J53" t="s">
-        <v>137</v>
-      </c>
-      <c r="K53" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B54" t="s">
         <v>100</v>
@@ -4298,33 +4286,33 @@
         <v>91</v>
       </c>
       <c r="D54" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="E54" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="F54" t="s">
         <v>96</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="G54" s="1">
+        <v>45642</v>
+      </c>
+      <c r="H54" s="1">
+        <v>45658</v>
+      </c>
+      <c r="I54" t="s">
+        <v>130</v>
+      </c>
+      <c r="J54" t="s">
+        <v>137</v>
+      </c>
+      <c r="K54" t="s">
         <v>157</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I54" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J54" t="s">
-        <v>137</v>
-      </c>
-      <c r="K54" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B55" t="s">
         <v>100</v>
@@ -4333,45 +4321,45 @@
         <v>91</v>
       </c>
       <c r="D55" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="E55" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="F55" t="s">
         <v>96</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G55" s="1">
+        <v>45647</v>
+      </c>
+      <c r="H55" s="1">
+        <v>45647</v>
+      </c>
+      <c r="I55" t="s">
+        <v>130</v>
+      </c>
+      <c r="J55" t="s">
+        <v>131</v>
+      </c>
+      <c r="K55" t="s">
         <v>157</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I55" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J55" t="s">
-        <v>137</v>
-      </c>
-      <c r="K55" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B56" t="s">
         <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D56" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E56" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="F56" t="s">
         <v>96</v>
@@ -4379,55 +4367,55 @@
       <c r="G56" s="1">
         <v>45647</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H56" s="1">
+        <v>45647</v>
+      </c>
+      <c r="I56" t="s">
+        <v>130</v>
+      </c>
+      <c r="J56" t="s">
+        <v>149</v>
+      </c>
+      <c r="K56" t="s">
         <v>157</v>
       </c>
-      <c r="I56" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J56" t="s">
-        <v>137</v>
-      </c>
-      <c r="K56" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>1424749</v>
+        <v>1421048</v>
       </c>
       <c r="B57" t="s">
         <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D57" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E57" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="F57" t="s">
         <v>96</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="G57" s="1">
+        <v>45647</v>
+      </c>
+      <c r="H57" s="1">
+        <v>45647</v>
+      </c>
+      <c r="I57" t="s">
+        <v>138</v>
+      </c>
+      <c r="J57" t="s">
+        <v>150</v>
+      </c>
+      <c r="K57" t="s">
         <v>157</v>
       </c>
-      <c r="H57" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I57" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J57" t="s">
-        <v>137</v>
-      </c>
-      <c r="K57" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1424749</v>
       </c>
@@ -4435,34 +4423,34 @@
         <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D58" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E58" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="F58" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="1" t="s">
-        <v>157</v>
+      <c r="G58" s="1">
+        <v>45644</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I58" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I58" t="s">
+        <v>134</v>
       </c>
       <c r="J58" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="K58" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1424749</v>
       </c>
@@ -4470,34 +4458,31 @@
         <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D59" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E59" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="F59" t="s">
         <v>96</v>
       </c>
-      <c r="G59" s="1" t="s">
-        <v>157</v>
+      <c r="G59" s="1">
+        <v>45646</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I59" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I59" t="s">
+        <v>136</v>
       </c>
       <c r="J59" t="s">
         <v>137</v>
       </c>
-      <c r="K59" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1424749</v>
       </c>
@@ -4505,34 +4490,31 @@
         <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D60" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E60" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="F60" t="s">
         <v>96</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I60" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I60" t="s">
+        <v>136</v>
       </c>
       <c r="J60" t="s">
         <v>137</v>
       </c>
-      <c r="K60" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1424749</v>
       </c>
@@ -4540,34 +4522,31 @@
         <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D61" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E61" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F61" t="s">
         <v>96</v>
       </c>
-      <c r="G61" s="1" t="s">
-        <v>157</v>
+      <c r="G61" s="1">
+        <v>45706</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I61" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I61" t="s">
+        <v>136</v>
       </c>
       <c r="J61" t="s">
-        <v>137</v>
-      </c>
-      <c r="K61" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1424749</v>
       </c>
@@ -4578,31 +4557,28 @@
         <v>91</v>
       </c>
       <c r="D62" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E62" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="F62" t="s">
         <v>96</v>
       </c>
-      <c r="G62" s="1">
-        <v>45644</v>
+      <c r="G62" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I62" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I62" t="s">
+        <v>136</v>
       </c>
       <c r="J62" t="s">
         <v>137</v>
       </c>
-      <c r="K62" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1424749</v>
       </c>
@@ -4613,10 +4589,10 @@
         <v>91</v>
       </c>
       <c r="D63" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E63" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F63" t="s">
         <v>96</v>
@@ -4624,20 +4600,17 @@
       <c r="G63" s="1">
         <v>45647</v>
       </c>
-      <c r="H63" s="1">
-        <v>45658</v>
-      </c>
-      <c r="I63" s="1">
-        <v>45642</v>
+      <c r="H63" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I63" t="s">
+        <v>136</v>
       </c>
       <c r="J63" t="s">
-        <v>139</v>
-      </c>
-      <c r="K63" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1424749</v>
       </c>
@@ -4648,31 +4621,28 @@
         <v>91</v>
       </c>
       <c r="D64" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="E64" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="F64" t="s">
         <v>96</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I64" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I64" t="s">
+        <v>136</v>
       </c>
       <c r="J64" t="s">
         <v>137</v>
       </c>
-      <c r="K64" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1424749</v>
       </c>
@@ -4683,31 +4653,28 @@
         <v>91</v>
       </c>
       <c r="D65" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="E65" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="F65" t="s">
         <v>96</v>
       </c>
-      <c r="G65" s="1">
-        <v>45647</v>
+      <c r="G65" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I65" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I65" t="s">
+        <v>136</v>
       </c>
       <c r="J65" t="s">
         <v>137</v>
       </c>
-      <c r="K65" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1424749</v>
       </c>
@@ -4718,313 +4685,289 @@
         <v>91</v>
       </c>
       <c r="D66" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="E66" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="F66" t="s">
         <v>96</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G66" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I66" t="s">
+        <v>136</v>
+      </c>
+      <c r="J66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>1424749</v>
+      </c>
+      <c r="B67" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" t="s">
+        <v>111</v>
+      </c>
+      <c r="E67" t="s">
+        <v>112</v>
+      </c>
+      <c r="F67" t="s">
+        <v>96</v>
+      </c>
+      <c r="G67" s="1">
         <v>45647</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="H67" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I67" t="s">
+        <v>136</v>
+      </c>
+      <c r="J67" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>1424749</v>
+      </c>
+      <c r="B68" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68" t="s">
+        <v>111</v>
+      </c>
+      <c r="E68" t="s">
+        <v>113</v>
+      </c>
+      <c r="F68" t="s">
+        <v>96</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I68" t="s">
+        <v>136</v>
+      </c>
+      <c r="J68" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>1424749</v>
+      </c>
+      <c r="B69" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" t="s">
+        <v>111</v>
+      </c>
+      <c r="E69" t="s">
+        <v>114</v>
+      </c>
+      <c r="F69" t="s">
+        <v>96</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I69" t="s">
+        <v>136</v>
+      </c>
+      <c r="J69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1424749</v>
+      </c>
+      <c r="B70" t="s">
+        <v>100</v>
+      </c>
+      <c r="C70" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" t="s">
+        <v>111</v>
+      </c>
+      <c r="E70" t="s">
+        <v>115</v>
+      </c>
+      <c r="F70" t="s">
+        <v>96</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I70" t="s">
+        <v>136</v>
+      </c>
+      <c r="J70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>1424749</v>
+      </c>
+      <c r="B71" t="s">
+        <v>100</v>
+      </c>
+      <c r="C71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" t="s">
+        <v>111</v>
+      </c>
+      <c r="E71" t="s">
+        <v>116</v>
+      </c>
+      <c r="F71" t="s">
+        <v>96</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I71" t="s">
+        <v>136</v>
+      </c>
+      <c r="J71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>1424749</v>
+      </c>
+      <c r="B72" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" t="s">
+        <v>111</v>
+      </c>
+      <c r="E72" t="s">
+        <v>117</v>
+      </c>
+      <c r="F72" t="s">
+        <v>96</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I72" t="s">
+        <v>136</v>
+      </c>
+      <c r="J72" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>1424749</v>
+      </c>
+      <c r="B73" t="s">
+        <v>100</v>
+      </c>
+      <c r="C73" t="s">
+        <v>91</v>
+      </c>
+      <c r="D73" t="s">
+        <v>118</v>
+      </c>
+      <c r="E73" t="s">
+        <v>119</v>
+      </c>
+      <c r="F73" t="s">
+        <v>96</v>
+      </c>
+      <c r="G73" s="1">
+        <v>45644</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I73" t="s">
+        <v>136</v>
+      </c>
+      <c r="J73" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>1424749</v>
+      </c>
+      <c r="B74" t="s">
+        <v>100</v>
+      </c>
+      <c r="C74" t="s">
+        <v>91</v>
+      </c>
+      <c r="D74" t="s">
+        <v>118</v>
+      </c>
+      <c r="E74" t="s">
+        <v>120</v>
+      </c>
+      <c r="F74" t="s">
+        <v>96</v>
+      </c>
+      <c r="G74" s="1">
+        <v>45647</v>
+      </c>
+      <c r="H74" s="1">
+        <v>45658</v>
+      </c>
+      <c r="I74" t="s">
+        <v>138</v>
+      </c>
+      <c r="J74" t="s">
+        <v>137</v>
+      </c>
+      <c r="K74" t="s">
         <v>157</v>
       </c>
-      <c r="I66" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J66" t="s">
-        <v>137</v>
-      </c>
-      <c r="K66" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>1424775</v>
-      </c>
-      <c r="B67" t="s">
-        <v>100</v>
-      </c>
-      <c r="C67" t="s">
-        <v>91</v>
-      </c>
-      <c r="D67" t="s">
-        <v>101</v>
-      </c>
-      <c r="E67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F67" t="s">
-        <v>95</v>
-      </c>
-      <c r="G67" t="s">
-        <v>157</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I67" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J67" t="s">
-        <v>150</v>
-      </c>
-      <c r="K67" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>1424775</v>
-      </c>
-      <c r="B68" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" t="s">
-        <v>91</v>
-      </c>
-      <c r="D68" t="s">
-        <v>101</v>
-      </c>
-      <c r="E68" t="s">
-        <v>103</v>
-      </c>
-      <c r="F68" t="s">
-        <v>95</v>
-      </c>
-      <c r="G68" t="s">
-        <v>157</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I68" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J68" t="s">
-        <v>137</v>
-      </c>
-      <c r="K68" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>1424775</v>
-      </c>
-      <c r="B69" t="s">
-        <v>100</v>
-      </c>
-      <c r="C69" t="s">
-        <v>91</v>
-      </c>
-      <c r="D69" t="s">
-        <v>101</v>
-      </c>
-      <c r="E69" t="s">
-        <v>104</v>
-      </c>
-      <c r="F69" t="s">
-        <v>95</v>
-      </c>
-      <c r="G69" t="s">
-        <v>157</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I69" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J69" t="s">
-        <v>137</v>
-      </c>
-      <c r="K69" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>1424775</v>
-      </c>
-      <c r="B70" t="s">
-        <v>100</v>
-      </c>
-      <c r="C70" t="s">
-        <v>91</v>
-      </c>
-      <c r="D70" t="s">
-        <v>101</v>
-      </c>
-      <c r="E70" t="s">
-        <v>105</v>
-      </c>
-      <c r="F70" t="s">
-        <v>95</v>
-      </c>
-      <c r="G70" t="s">
-        <v>157</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I70" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J70" t="s">
-        <v>150</v>
-      </c>
-      <c r="K70" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>1424775</v>
-      </c>
-      <c r="B71" t="s">
-        <v>100</v>
-      </c>
-      <c r="C71" t="s">
-        <v>91</v>
-      </c>
-      <c r="D71" t="s">
-        <v>101</v>
-      </c>
-      <c r="E71" t="s">
-        <v>106</v>
-      </c>
-      <c r="F71" t="s">
-        <v>95</v>
-      </c>
-      <c r="G71" t="s">
-        <v>157</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I71" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J71" t="s">
-        <v>137</v>
-      </c>
-      <c r="K71" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>1424775</v>
-      </c>
-      <c r="B72" t="s">
-        <v>100</v>
-      </c>
-      <c r="C72" t="s">
-        <v>91</v>
-      </c>
-      <c r="D72" t="s">
-        <v>101</v>
-      </c>
-      <c r="E72" t="s">
-        <v>107</v>
-      </c>
-      <c r="F72" t="s">
-        <v>95</v>
-      </c>
-      <c r="G72" t="s">
-        <v>157</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I72" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J72" t="s">
-        <v>137</v>
-      </c>
-      <c r="K72" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>1424775</v>
-      </c>
-      <c r="B73" t="s">
-        <v>100</v>
-      </c>
-      <c r="C73" t="s">
-        <v>91</v>
-      </c>
-      <c r="D73" t="s">
-        <v>101</v>
-      </c>
-      <c r="E73" t="s">
-        <v>108</v>
-      </c>
-      <c r="F73" t="s">
-        <v>95</v>
-      </c>
-      <c r="G73" t="s">
-        <v>157</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I73" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J73" t="s">
-        <v>137</v>
-      </c>
-      <c r="K73" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>1424775</v>
-      </c>
-      <c r="B74" t="s">
-        <v>100</v>
-      </c>
-      <c r="C74" t="s">
-        <v>91</v>
-      </c>
-      <c r="D74" t="s">
-        <v>101</v>
-      </c>
-      <c r="E74" t="s">
-        <v>109</v>
-      </c>
-      <c r="F74" t="s">
-        <v>95</v>
-      </c>
-      <c r="G74" t="s">
-        <v>157</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I74" s="1">
-        <v>45642</v>
-      </c>
-      <c r="J74" t="s">
-        <v>137</v>
-      </c>
-      <c r="K74" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>1424775</v>
+        <v>1424749</v>
       </c>
       <c r="B75" t="s">
         <v>100</v>
@@ -5033,33 +4976,30 @@
         <v>91</v>
       </c>
       <c r="D75" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="E75" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="F75" t="s">
-        <v>95</v>
-      </c>
-      <c r="G75" t="s">
-        <v>157</v>
+        <v>96</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I75" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I75" t="s">
+        <v>136</v>
       </c>
       <c r="J75" t="s">
         <v>137</v>
       </c>
-      <c r="K75" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>1424775</v>
+        <v>1424749</v>
       </c>
       <c r="B76" t="s">
         <v>100</v>
@@ -5068,33 +5008,33 @@
         <v>91</v>
       </c>
       <c r="D76" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E76" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F76" t="s">
-        <v>94</v>
-      </c>
-      <c r="G76" t="s">
-        <v>157</v>
+        <v>96</v>
+      </c>
+      <c r="G76" s="1">
+        <v>45647</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I76" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I76" t="s">
+        <v>134</v>
       </c>
       <c r="J76" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="K76" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>1424775</v>
+        <v>1424749</v>
       </c>
       <c r="B77" t="s">
         <v>100</v>
@@ -5103,33 +5043,30 @@
         <v>91</v>
       </c>
       <c r="D77" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E77" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F77" t="s">
-        <v>94</v>
-      </c>
-      <c r="G77" t="s">
-        <v>157</v>
+        <v>96</v>
+      </c>
+      <c r="G77" s="1">
+        <v>45647</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I77" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I77" t="s">
+        <v>136</v>
       </c>
       <c r="J77" t="s">
-        <v>137</v>
-      </c>
-      <c r="K77" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>1424775</v>
+        <v>1424749</v>
       </c>
       <c r="B78" t="s">
         <v>100</v>
@@ -5138,33 +5075,33 @@
         <v>91</v>
       </c>
       <c r="D78" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="E78" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="F78" t="s">
         <v>96</v>
       </c>
-      <c r="G78" t="s">
-        <v>157</v>
+      <c r="G78" s="1">
+        <v>45810</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I78" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I78" t="s">
+        <v>134</v>
       </c>
       <c r="J78" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="K78" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>1424775</v>
+        <v>1424749</v>
       </c>
       <c r="B79" t="s">
         <v>100</v>
@@ -5173,33 +5110,30 @@
         <v>91</v>
       </c>
       <c r="D79" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="E79" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="F79" t="s">
         <v>96</v>
       </c>
-      <c r="G79" t="s">
-        <v>157</v>
+      <c r="G79" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I79" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I79" t="s">
+        <v>136</v>
       </c>
       <c r="J79" t="s">
         <v>137</v>
       </c>
-      <c r="K79" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>1424775</v>
+        <v>1424749</v>
       </c>
       <c r="B80" t="s">
         <v>100</v>
@@ -5208,32 +5142,660 @@
         <v>91</v>
       </c>
       <c r="D80" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="E80" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="F80" t="s">
         <v>96</v>
       </c>
-      <c r="G80" t="s">
-        <v>157</v>
+      <c r="G80" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I80" s="1">
-        <v>45642</v>
+        <v>155</v>
+      </c>
+      <c r="I80" t="s">
+        <v>148</v>
       </c>
       <c r="J80" t="s">
         <v>137</v>
       </c>
       <c r="K80" t="s">
-        <v>138</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>1424749</v>
+      </c>
+      <c r="B81" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" t="s">
+        <v>91</v>
+      </c>
+      <c r="D81" t="s">
+        <v>158</v>
+      </c>
+      <c r="E81" t="s">
+        <v>165</v>
+      </c>
+      <c r="F81" t="s">
+        <v>96</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I81" t="s">
+        <v>136</v>
+      </c>
+      <c r="J81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>1424749</v>
+      </c>
+      <c r="B82" t="s">
+        <v>100</v>
+      </c>
+      <c r="C82" t="s">
+        <v>91</v>
+      </c>
+      <c r="D82" t="s">
+        <v>158</v>
+      </c>
+      <c r="E82" t="s">
+        <v>167</v>
+      </c>
+      <c r="F82" t="s">
+        <v>96</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I82" t="s">
+        <v>136</v>
+      </c>
+      <c r="J82" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1424749</v>
+      </c>
+      <c r="B83" t="s">
+        <v>100</v>
+      </c>
+      <c r="C83" t="s">
+        <v>91</v>
+      </c>
+      <c r="D83" t="s">
+        <v>158</v>
+      </c>
+      <c r="E83" t="s">
+        <v>168</v>
+      </c>
+      <c r="F83" t="s">
+        <v>96</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I83" t="s">
+        <v>148</v>
+      </c>
+      <c r="J83" t="s">
+        <v>137</v>
+      </c>
+      <c r="K83" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1424749</v>
+      </c>
+      <c r="B84" t="s">
+        <v>100</v>
+      </c>
+      <c r="C84" t="s">
+        <v>91</v>
+      </c>
+      <c r="D84" t="s">
+        <v>158</v>
+      </c>
+      <c r="E84" t="s">
+        <v>170</v>
+      </c>
+      <c r="F84" t="s">
+        <v>96</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I84" t="s">
+        <v>171</v>
+      </c>
+      <c r="J84" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1424749</v>
+      </c>
+      <c r="B85" t="s">
+        <v>100</v>
+      </c>
+      <c r="C85" t="s">
+        <v>91</v>
+      </c>
+      <c r="D85" t="s">
+        <v>158</v>
+      </c>
+      <c r="E85" t="s">
+        <v>172</v>
+      </c>
+      <c r="F85" t="s">
+        <v>96</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I85" t="s">
+        <v>148</v>
+      </c>
+      <c r="J85" t="s">
+        <v>137</v>
+      </c>
+      <c r="K85" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1424775</v>
+      </c>
+      <c r="B86" t="s">
+        <v>100</v>
+      </c>
+      <c r="C86" t="s">
+        <v>91</v>
+      </c>
+      <c r="D86" t="s">
+        <v>101</v>
+      </c>
+      <c r="E86" t="s">
+        <v>102</v>
+      </c>
+      <c r="F86" t="s">
+        <v>95</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I86" t="s">
+        <v>148</v>
+      </c>
+      <c r="J86" t="s">
+        <v>137</v>
+      </c>
+      <c r="K86" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1424775</v>
+      </c>
+      <c r="B87" t="s">
+        <v>100</v>
+      </c>
+      <c r="C87" t="s">
+        <v>91</v>
+      </c>
+      <c r="D87" t="s">
+        <v>101</v>
+      </c>
+      <c r="E87" t="s">
+        <v>103</v>
+      </c>
+      <c r="F87" t="s">
+        <v>95</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I87" t="s">
+        <v>136</v>
+      </c>
+      <c r="J87" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1424775</v>
+      </c>
+      <c r="B88" t="s">
+        <v>100</v>
+      </c>
+      <c r="C88" t="s">
+        <v>91</v>
+      </c>
+      <c r="D88" t="s">
+        <v>101</v>
+      </c>
+      <c r="E88" t="s">
+        <v>104</v>
+      </c>
+      <c r="F88" t="s">
+        <v>95</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I88" t="s">
+        <v>136</v>
+      </c>
+      <c r="J88" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1424775</v>
+      </c>
+      <c r="B89" t="s">
+        <v>100</v>
+      </c>
+      <c r="C89" t="s">
+        <v>91</v>
+      </c>
+      <c r="D89" t="s">
+        <v>101</v>
+      </c>
+      <c r="E89" t="s">
+        <v>105</v>
+      </c>
+      <c r="F89" t="s">
+        <v>95</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I89" t="s">
+        <v>136</v>
+      </c>
+      <c r="J89" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1424775</v>
+      </c>
+      <c r="B90" t="s">
+        <v>100</v>
+      </c>
+      <c r="C90" t="s">
+        <v>91</v>
+      </c>
+      <c r="D90" t="s">
+        <v>101</v>
+      </c>
+      <c r="E90" t="s">
+        <v>106</v>
+      </c>
+      <c r="F90" t="s">
+        <v>95</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I90" t="s">
+        <v>136</v>
+      </c>
+      <c r="J90" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>1424775</v>
+      </c>
+      <c r="B91" t="s">
+        <v>100</v>
+      </c>
+      <c r="C91" t="s">
+        <v>91</v>
+      </c>
+      <c r="D91" t="s">
+        <v>101</v>
+      </c>
+      <c r="E91" t="s">
+        <v>107</v>
+      </c>
+      <c r="F91" t="s">
+        <v>95</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I91" t="s">
+        <v>136</v>
+      </c>
+      <c r="J91" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1424775</v>
+      </c>
+      <c r="B92" t="s">
+        <v>100</v>
+      </c>
+      <c r="C92" t="s">
+        <v>91</v>
+      </c>
+      <c r="D92" t="s">
+        <v>101</v>
+      </c>
+      <c r="E92" t="s">
+        <v>108</v>
+      </c>
+      <c r="F92" t="s">
+        <v>95</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I92" t="s">
+        <v>136</v>
+      </c>
+      <c r="J92" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1424775</v>
+      </c>
+      <c r="B93" t="s">
+        <v>100</v>
+      </c>
+      <c r="C93" t="s">
+        <v>91</v>
+      </c>
+      <c r="D93" t="s">
+        <v>101</v>
+      </c>
+      <c r="E93" t="s">
+        <v>109</v>
+      </c>
+      <c r="F93" t="s">
+        <v>95</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I93" t="s">
+        <v>136</v>
+      </c>
+      <c r="J93" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1424775</v>
+      </c>
+      <c r="B94" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94" t="s">
+        <v>91</v>
+      </c>
+      <c r="D94" t="s">
+        <v>101</v>
+      </c>
+      <c r="E94" t="s">
+        <v>110</v>
+      </c>
+      <c r="F94" t="s">
+        <v>95</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I94" t="s">
+        <v>136</v>
+      </c>
+      <c r="J94" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>1424775</v>
+      </c>
+      <c r="B95" t="s">
+        <v>100</v>
+      </c>
+      <c r="C95" t="s">
+        <v>91</v>
+      </c>
+      <c r="D95" t="s">
+        <v>118</v>
+      </c>
+      <c r="E95" t="s">
+        <v>119</v>
+      </c>
+      <c r="F95" t="s">
+        <v>94</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I95" t="s">
+        <v>136</v>
+      </c>
+      <c r="J95" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>1424775</v>
+      </c>
+      <c r="B96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96" t="s">
+        <v>91</v>
+      </c>
+      <c r="D96" t="s">
+        <v>118</v>
+      </c>
+      <c r="E96" t="s">
+        <v>120</v>
+      </c>
+      <c r="F96" t="s">
+        <v>94</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I96" t="s">
+        <v>136</v>
+      </c>
+      <c r="J96" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>1424775</v>
+      </c>
+      <c r="B97" t="s">
+        <v>100</v>
+      </c>
+      <c r="C97" t="s">
+        <v>91</v>
+      </c>
+      <c r="D97" t="s">
+        <v>121</v>
+      </c>
+      <c r="E97" t="s">
+        <v>122</v>
+      </c>
+      <c r="F97" t="s">
+        <v>96</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I97" t="s">
+        <v>136</v>
+      </c>
+      <c r="J97" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>1424775</v>
+      </c>
+      <c r="B98" t="s">
+        <v>100</v>
+      </c>
+      <c r="C98" t="s">
+        <v>91</v>
+      </c>
+      <c r="D98" t="s">
+        <v>123</v>
+      </c>
+      <c r="E98" t="s">
+        <v>124</v>
+      </c>
+      <c r="F98" t="s">
+        <v>96</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I98" t="s">
+        <v>171</v>
+      </c>
+      <c r="J98" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>1424775</v>
+      </c>
+      <c r="B99" t="s">
+        <v>100</v>
+      </c>
+      <c r="C99" t="s">
+        <v>91</v>
+      </c>
+      <c r="D99" t="s">
+        <v>123</v>
+      </c>
+      <c r="E99" t="s">
+        <v>125</v>
+      </c>
+      <c r="F99" t="s">
+        <v>96</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I99" t="s">
+        <v>136</v>
+      </c>
+      <c r="J99" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H80" xr:uid="{4DEF9A41-F379-1F49-B5CE-AAD7CB2EE5A6}"/>
+  <autoFilter ref="A1:K99" xr:uid="{4DEF9A41-F379-1F49-B5CE-AAD7CB2EE5A6}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="1421046"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Trilha 8 - Todos Status de Módulo"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>